<commit_message>
getting all rows and layout for them
</commit_message>
<xml_diff>
--- a/reported hours/Reported hours - Jonathan Larsson.xlsx
+++ b/reported hours/Reported hours - Jonathan Larsson.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Airkick/Documents/Årskurs 3/Software Engineering Project/DVA313-Solar-Energy/reported hours/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/DVA313-Solar-Energy/reported hours/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -632,7 +632,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -668,7 +668,7 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working default upload, update and download
</commit_message>
<xml_diff>
--- a/reported hours/Reported hours - Jonathan Larsson.xlsx
+++ b/reported hours/Reported hours - Jonathan Larsson.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
   <si>
     <t>Reported hours for:</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>Presentation</t>
+  </si>
+  <si>
+    <t>implementation</t>
+  </si>
+  <si>
+    <t>Project presentation</t>
+  </si>
+  <si>
+    <t>Excel creation</t>
   </si>
 </sst>
 </file>
@@ -633,10 +642,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -681,6 +690,30 @@
       </c>
       <c r="B5">
         <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug that was seen during client meeting
</commit_message>
<xml_diff>
--- a/reported hours/Reported hours - Jonathan Larsson.xlsx
+++ b/reported hours/Reported hours - Jonathan Larsson.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15360" windowHeight="10480" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15360" windowHeight="10480" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="20">
   <si>
     <t>Reported hours for:</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t>Excel upload</t>
+  </si>
+  <si>
+    <t>meetings</t>
+  </si>
+  <si>
+    <t>gui</t>
+  </si>
+  <si>
+    <t>design description</t>
   </si>
 </sst>
 </file>
@@ -647,7 +656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -741,9 +750,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -763,6 +774,30 @@
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change default menu tabs for admin and user
</commit_message>
<xml_diff>
--- a/reported hours/Reported hours - Jonathan Larsson.xlsx
+++ b/reported hours/Reported hours - Jonathan Larsson.xlsx
@@ -753,7 +753,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -789,7 +789,7 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
@@ -797,7 +797,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
column b, c, g calculations
</commit_message>
<xml_diff>
--- a/reported hours/Reported hours - Jonathan Larsson.xlsx
+++ b/reported hours/Reported hours - Jonathan Larsson.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15360" windowHeight="10480" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15360" windowHeight="10480" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="22">
   <si>
     <t>Reported hours for:</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>design description</t>
+  </si>
+  <si>
+    <t>presentation</t>
+  </si>
+  <si>
+    <t>presentation prep</t>
   </si>
 </sst>
 </file>
@@ -752,7 +758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -822,9 +828,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -844,6 +852,38 @@
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finally done with integration
</commit_message>
<xml_diff>
--- a/reported hours/Reported hours - Jonathan Larsson.xlsx
+++ b/reported hours/Reported hours - Jonathan Larsson.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15360" windowHeight="10480" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15360" windowHeight="10480" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="22">
   <si>
     <t>Reported hours for:</t>
   </si>
@@ -830,7 +830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -900,9 +900,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -922,6 +924,14 @@
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new toLocaleString function and download pdf instead of open
</commit_message>
<xml_diff>
--- a/reported hours/Reported hours - Jonathan Larsson.xlsx
+++ b/reported hours/Reported hours - Jonathan Larsson.xlsx
@@ -567,7 +567,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -595,7 +595,7 @@
         <v>23</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hidden login and changed to swedish login modal
</commit_message>
<xml_diff>
--- a/reported hours/Reported hours - Jonathan Larsson.xlsx
+++ b/reported hours/Reported hours - Jonathan Larsson.xlsx
@@ -567,7 +567,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -595,7 +595,7 @@
         <v>23</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>